<commit_message>
Servo is working, tbd: init motors
</commit_message>
<xml_diff>
--- a/doc/pinout.xlsx
+++ b/doc/pinout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vutbr-my.sharepoint.com/personal/xjahnf00_vutbr_cz/Documents/Bakalarska prace/Workspace/doc/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Windows.old\Users\filip\Documents\MCUXpressoIDE_11.5.1_7266\workspace\frdmkl25z\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{2FA1FDBF-BAC6-4C96-95F4-04737D09B01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67D1DF56-8648-41FA-9A63-B31C53226CCA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C826F3D5-CB05-4E77-B9A1-9B5EFF5F7F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>https://www.openhacks.com/uploadsproductos/frdm-kl25z_pinouts__rev_1.0_.pdf</t>
   </si>
   <si>
-    <t>PTE25</t>
-  </si>
-  <si>
     <t>Servo motor</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>FTM1_CH0</t>
   </si>
   <si>
-    <t>FTM0_CH1</t>
-  </si>
-  <si>
     <t>Left color sensor</t>
   </si>
   <si>
@@ -220,6 +214,12 @@
   </si>
   <si>
     <t>GPIOA, 4</t>
+  </si>
+  <si>
+    <t>PTD5</t>
+  </si>
+  <si>
+    <t>FTM0_CH5</t>
   </si>
 </sst>
 </file>
@@ -837,24 +837,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="22"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="10" max="10" width="76.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="22"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="1"/>
+    <col min="10" max="10" width="76.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -862,24 +862,24 @@
       <c r="F2" s="26"/>
       <c r="G2" s="27"/>
       <c r="J2" s="30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
@@ -888,7 +888,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
@@ -896,19 +896,19 @@
         <v>1</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="15"/>
       <c r="H4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
@@ -916,37 +916,37 @@
         <v>3</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="15"/>
       <c r="H5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="D6" s="11" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="12"/>
       <c r="H6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -955,9 +955,9 @@
       <c r="G7" s="1"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B8" s="25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
@@ -965,61 +965,61 @@
       <c r="F8" s="26"/>
       <c r="G8" s="27"/>
     </row>
-    <row r="9" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="18" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
-        <v>21</v>
-      </c>
       <c r="C11" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="14"/>
       <c r="G11" s="15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1027,9 +1027,9 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B13" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
@@ -1037,170 +1037,170 @@
       <c r="F13" s="26"/>
       <c r="G13" s="27"/>
     </row>
-    <row r="14" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="18" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C16" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="19" t="s">
+      <c r="D17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>13</v>
-      </c>
       <c r="D18" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>15</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1208,9 +1208,9 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B23" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
@@ -1218,51 +1218,51 @@
       <c r="F23" s="26"/>
       <c r="G23" s="27"/>
     </row>
-    <row r="24" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="28" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B28" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
@@ -1270,42 +1270,42 @@
       <c r="F28" s="26"/>
       <c r="G28" s="27"/>
     </row>
-    <row r="29" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>

</xml_diff>

<commit_message>
Edit: I2C0, Fix: i2cInit, sensor still not working
</commit_message>
<xml_diff>
--- a/doc/pinout.xlsx
+++ b/doc/pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Windows.old\Users\filip\Documents\MCUXpressoIDE_11.5.1_7266\workspace\frdmkl25z\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C826F3D5-CB05-4E77-B9A1-9B5EFF5F7F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996AE6EE-ABAD-48AB-AA30-22F69B0A1C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,12 +99,6 @@
     <t>Laser</t>
   </si>
   <si>
-    <t>PTC11</t>
-  </si>
-  <si>
-    <t>PTC10</t>
-  </si>
-  <si>
     <t>I2C1</t>
   </si>
   <si>
@@ -220,6 +214,12 @@
   </si>
   <si>
     <t>FTM0_CH5</t>
+  </si>
+  <si>
+    <t>PTC9</t>
+  </si>
+  <si>
+    <t>PTC8</t>
   </si>
 </sst>
 </file>
@@ -837,22 +837,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="1"/>
-    <col min="10" max="10" width="76.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="10" max="10" width="76.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
         <v>21</v>
       </c>
@@ -862,24 +862,24 @@
       <c r="F2" s="26"/>
       <c r="G2" s="27"/>
       <c r="J2" s="30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
@@ -888,7 +888,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
@@ -902,13 +902,13 @@
       <c r="F4" s="14"/>
       <c r="G4" s="15"/>
       <c r="H4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
@@ -922,31 +922,31 @@
       <c r="F5" s="14"/>
       <c r="G5" s="15"/>
       <c r="H5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="12"/>
       <c r="H6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -955,9 +955,9 @@
       <c r="G7" s="1"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="2:13" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
@@ -965,31 +965,31 @@
       <c r="F8" s="26"/>
       <c r="G8" s="27"/>
     </row>
-    <row r="9" spans="2:13" ht="18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -1000,15 +1000,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="14"/>
@@ -1019,7 +1019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1027,7 +1027,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:13" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
         <v>22</v>
       </c>
@@ -1037,66 +1037,66 @@
       <c r="F13" s="26"/>
       <c r="G13" s="27"/>
     </row>
-    <row r="14" spans="2:13" ht="18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>20</v>
       </c>
@@ -1104,27 +1104,27 @@
         <v>10</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>16</v>
@@ -1137,7 +1137,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>18</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>16</v>
@@ -1158,49 +1158,49 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1208,7 +1208,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
         <v>23</v>
       </c>
@@ -1218,51 +1218,51 @@
       <c r="F23" s="26"/>
       <c r="G23" s="27"/>
     </row>
-    <row r="24" spans="2:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="28" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
@@ -1270,42 +1270,42 @@
       <c r="F28" s="26"/>
       <c r="G28" s="27"/>
     </row>
-    <row r="29" spans="2:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>

</xml_diff>

<commit_message>
Change pinouts, add SD
</commit_message>
<xml_diff>
--- a/doc/pinout.xlsx
+++ b/doc/pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Windows.old\Users\filip\Documents\MCUXpressoIDE_11.5.1_7266\workspace\frdmkl25z\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A97AC60-B440-43CC-916F-3D85079E7F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E805A9D-8370-4ABA-B36A-7C904B6C1FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>PTA13</t>
   </si>
@@ -60,30 +60,12 @@
     <t>Center color sensor</t>
   </si>
   <si>
-    <t>Left helping sensor</t>
-  </si>
-  <si>
-    <t>Right helping sensor</t>
-  </si>
-  <si>
-    <t>S0, S2 TCS3200 pin</t>
-  </si>
-  <si>
-    <t>S1, S3 TCS3200 pin</t>
-  </si>
-  <si>
     <t xml:space="preserve"> TCS3200</t>
   </si>
   <si>
-    <t>Todo</t>
-  </si>
-  <si>
     <t>IRQ</t>
   </si>
   <si>
-    <t>PTA5</t>
-  </si>
-  <si>
     <t>PTD2</t>
   </si>
   <si>
@@ -96,15 +78,6 @@
     <t>Senzory</t>
   </si>
   <si>
-    <t>Laser</t>
-  </si>
-  <si>
-    <t>PTC11</t>
-  </si>
-  <si>
-    <t>PTC10</t>
-  </si>
-  <si>
     <t>I2C1</t>
   </si>
   <si>
@@ -126,15 +99,9 @@
     <t>PTA1</t>
   </si>
   <si>
-    <t>Left hall</t>
-  </si>
-  <si>
     <t>Right hall</t>
   </si>
   <si>
-    <t>HIGH</t>
-  </si>
-  <si>
     <t>LOW</t>
   </si>
   <si>
@@ -195,38 +162,50 @@
     <t>PWM</t>
   </si>
   <si>
-    <t>GPIO</t>
-  </si>
-  <si>
     <t>PTA2</t>
   </si>
   <si>
-    <t>GPIOC, 4</t>
-  </si>
-  <si>
-    <t>GPIOC, 5</t>
-  </si>
-  <si>
-    <t>GPIOA, 5</t>
-  </si>
-  <si>
-    <t>PTA4</t>
-  </si>
-  <si>
-    <t>GPIOA, 4</t>
-  </si>
-  <si>
     <t>PTD5</t>
   </si>
   <si>
     <t>FTM0_CH5</t>
+  </si>
+  <si>
+    <t>PTC7</t>
+  </si>
+  <si>
+    <t>PTC2</t>
+  </si>
+  <si>
+    <t>PTC1</t>
+  </si>
+  <si>
+    <t>Arduino (laser + adc)</t>
+  </si>
+  <si>
+    <t>PTC6</t>
+  </si>
+  <si>
+    <t>SD slot SPI</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>MOSI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,14 +228,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -286,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -411,16 +382,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -473,12 +478,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -504,6 +509,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -536,7 +560,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>333373</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -835,493 +859,475 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M31"/>
+  <dimension ref="A2:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="22"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="10" max="10" width="76.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="20"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="1"/>
+    <col min="10" max="10" width="76.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
+      <c r="J2" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
-      <c r="J2" s="30" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
+      <c r="D6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
       <c r="H6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="2:13" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B8" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="2:13" ht="18" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="31"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+    </row>
+    <row r="13" spans="2:13" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B13" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
+    </row>
+    <row r="14" spans="2:13" ht="18" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="E15" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="31"/>
+    </row>
+    <row r="19" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B19" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="31"/>
+    </row>
+    <row r="20" spans="2:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="31"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="31"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="23"/>
+    </row>
+    <row r="24" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B24" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="26"/>
+    </row>
+    <row r="25" spans="2:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="28"/>
+    </row>
+    <row r="29" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B29" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
+    </row>
+    <row r="30" spans="2:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="B30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C31" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-    </row>
-    <row r="14" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="19" t="s">
+      <c r="C32" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="19" t="s">
+      <c r="C33" s="18" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="24"/>
-    </row>
-    <row r="28" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="27"/>
-    </row>
-    <row r="29" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="28" t="s">
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="16" t="s">
+      <c r="C34" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="29"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="G30:G31"/>
+  <mergeCells count="9">
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="G26:G27"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>